<commit_message>
update bảng kế hoạch
</commit_message>
<xml_diff>
--- a/bảng kế  hoạch sau khi chỉnh sửa.xlsx
+++ b/bảng kế  hoạch sau khi chỉnh sửa.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanta\OneDrive\Documents\GitHub\CODE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vo Tan Nguyen\Documents\GitHub\CODE2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D738C7-4C7A-4D87-8336-BFD759B2ED2A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24990" windowHeight="7980"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24990" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>STT</t>
   </si>
@@ -155,7 +156,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -569,11 +570,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,8 +769,12 @@
       <c r="F8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="7"/>
+      <c r="G8" s="8">
+        <v>43400</v>
+      </c>
+      <c r="H8" s="8">
+        <v>43401</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
@@ -788,8 +793,12 @@
       <c r="F9" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="G9" s="8">
+        <v>43401</v>
+      </c>
+      <c r="H9" s="8">
+        <v>43401</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
@@ -806,10 +815,14 @@
         <v>20</v>
       </c>
       <c r="F10" s="8">
-        <v>43142</v>
-      </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+        <v>43406</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="8">
+        <v>43403</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
@@ -823,13 +836,17 @@
         <v>7</v>
       </c>
       <c r="E11" s="8">
-        <v>43170</v>
+        <v>43407</v>
       </c>
       <c r="F11" s="8">
-        <v>43201</v>
-      </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+        <v>43408</v>
+      </c>
+      <c r="G11" s="8">
+        <v>43405</v>
+      </c>
+      <c r="H11" s="8">
+        <v>43406</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
@@ -850,8 +867,12 @@
       <c r="F12" s="8">
         <v>43323</v>
       </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="8">
+        <v>43407</v>
+      </c>
+      <c r="H12" s="8">
+        <v>43407</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">

</xml_diff>